<commit_message>
Updating graphics + alhorithm
</commit_message>
<xml_diff>
--- a/out/dimension_1/deba1/stat.xlsx
+++ b/out/dimension_1/deba1/stat.xlsx
@@ -1047,10 +1047,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1600</v>
+        <v>37900</v>
       </c>
       <c r="C3">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1059,19 +1059,19 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>0.08928571428571429</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.9107142857142857</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K3">
-        <v>1800</v>
+        <v>36000</v>
       </c>
       <c r="L3">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="M3">
         <v>5</v>
@@ -1080,19 +1080,19 @@
         <v>5</v>
       </c>
       <c r="P3">
-        <v>0.18518518518518517</v>
+        <v>0.3125</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>0.8148148148148148</v>
+        <v>0.6875</v>
       </c>
       <c r="T3">
-        <v>2200</v>
+        <v>33900</v>
       </c>
       <c r="U3">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="V3">
         <v>5</v>
@@ -1101,19 +1101,19 @@
         <v>5</v>
       </c>
       <c r="Y3">
-        <v>0.15625</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AB3">
-        <v>0.84375</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="AC3">
-        <v>1700</v>
+        <v>30700</v>
       </c>
       <c r="AD3">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="AE3">
         <v>5</v>
@@ -1122,19 +1122,19 @@
         <v>5</v>
       </c>
       <c r="AH3">
-        <v>0.09615384615384616</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="AI3">
         <v>1</v>
       </c>
       <c r="AK3">
-        <v>0.9038461538461539</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="AL3">
-        <v>1700</v>
+        <v>31800</v>
       </c>
       <c r="AM3">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="AN3">
         <v>5</v>
@@ -1143,19 +1143,19 @@
         <v>5</v>
       </c>
       <c r="AQ3">
-        <v>0.10869565217391304</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="AR3">
         <v>1</v>
       </c>
       <c r="AT3">
-        <v>0.8913043478260869</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="AU3">
-        <v>1700</v>
+        <v>33500</v>
       </c>
       <c r="AV3">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="AW3">
         <v>5</v>
@@ -1164,40 +1164,40 @@
         <v>5</v>
       </c>
       <c r="AZ3">
-        <v>0.10416666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="BA3">
         <v>1</v>
       </c>
       <c r="BC3">
-        <v>0.8958333333333334</v>
+        <v>0.6875</v>
       </c>
       <c r="BD3">
-        <v>1800</v>
+        <v>40300</v>
       </c>
       <c r="BE3">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="BF3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BI3">
-        <v>0.12903225806451613</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="BJ3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="BL3">
-        <v>0.8709677419354839</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="BM3">
-        <v>1600</v>
+        <v>34700</v>
       </c>
       <c r="BN3">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="BO3">
         <v>5</v>
@@ -1206,19 +1206,19 @@
         <v>5</v>
       </c>
       <c r="BR3">
-        <v>0.09433962264150944</v>
+        <v>0.3125</v>
       </c>
       <c r="BS3">
         <v>1</v>
       </c>
       <c r="BU3">
-        <v>0.9056603773584906</v>
+        <v>0.6875</v>
       </c>
       <c r="BV3">
-        <v>1600</v>
+        <v>43200</v>
       </c>
       <c r="BW3">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="BX3">
         <v>5</v>
@@ -1227,19 +1227,19 @@
         <v>5</v>
       </c>
       <c r="CA3">
-        <v>0.09090909090909091</v>
+        <v>0.3125</v>
       </c>
       <c r="CB3">
         <v>1</v>
       </c>
       <c r="CD3">
-        <v>0.9090909090909091</v>
+        <v>0.6875</v>
       </c>
       <c r="CE3">
-        <v>1700</v>
+        <v>31500</v>
       </c>
       <c r="CF3">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="CG3">
         <v>5</v>
@@ -1248,46 +1248,46 @@
         <v>5</v>
       </c>
       <c r="CJ3">
-        <v>0.1111111111111111</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="CK3">
         <v>1</v>
       </c>
       <c r="CM3">
-        <v>0.8888888888888888</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="CN3">
-        <v>1740</v>
+        <v>35350</v>
       </c>
       <c r="CO3">
-        <v>44.5</v>
+        <v>16.2</v>
       </c>
       <c r="CP3">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CQ3">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CR3" t="str">
         <v/>
       </c>
       <c r="CS3">
-        <v>0.1165129147191553</v>
+        <v>0.3093137254901961</v>
       </c>
       <c r="CT3">
-        <v>0.9800000000000001</v>
+        <v>1</v>
       </c>
       <c r="CU3" t="str">
         <v/>
       </c>
       <c r="CV3">
-        <v>0.8834870852808446</v>
+        <v>0.690686274509804</v>
       </c>
       <c r="CW3">
-        <v>1600</v>
+        <v>30700</v>
       </c>
       <c r="CX3">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="CY3">
         <v>5</v>
@@ -1296,13 +1296,13 @@
         <v>5</v>
       </c>
       <c r="DB3">
-        <v>0.18518518518518517</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="DC3">
         <v>1</v>
       </c>
       <c r="DE3">
-        <v>0.8148148148148148</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="DF3">
         <v>100</v>
@@ -1313,10 +1313,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1500</v>
+        <v>19700</v>
       </c>
       <c r="C4">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1325,16 +1325,16 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <v>0.05952380952380952</v>
+        <v>0.08928571428571429</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.9404761904761905</v>
+        <v>0.9107142857142857</v>
       </c>
       <c r="K4">
-        <v>4500</v>
+        <v>13300</v>
       </c>
       <c r="L4">
         <v>49</v>
@@ -1355,10 +1355,10 @@
         <v>0.8979591836734694</v>
       </c>
       <c r="T4">
-        <v>1400</v>
+        <v>17500</v>
       </c>
       <c r="U4">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="V4">
         <v>5</v>
@@ -1367,19 +1367,19 @@
         <v>5</v>
       </c>
       <c r="Y4">
-        <v>0.06097560975609756</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="Z4">
         <v>1</v>
       </c>
       <c r="AB4">
-        <v>0.9390243902439024</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="AC4">
-        <v>1500</v>
+        <v>7600</v>
       </c>
       <c r="AD4">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="AE4">
         <v>5</v>
@@ -1388,19 +1388,19 @@
         <v>5</v>
       </c>
       <c r="AH4">
-        <v>0.0625</v>
+        <v>0.09615384615384616</v>
       </c>
       <c r="AI4">
         <v>1</v>
       </c>
       <c r="AK4">
-        <v>0.9375</v>
+        <v>0.9038461538461539</v>
       </c>
       <c r="AL4">
-        <v>1500</v>
+        <v>18800</v>
       </c>
       <c r="AM4">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="AN4">
         <v>5</v>
@@ -1409,19 +1409,19 @@
         <v>5</v>
       </c>
       <c r="AQ4">
-        <v>0.06493506493506493</v>
+        <v>0.08928571428571429</v>
       </c>
       <c r="AR4">
         <v>1</v>
       </c>
       <c r="AT4">
-        <v>0.935064935064935</v>
+        <v>0.9107142857142857</v>
       </c>
       <c r="AU4">
-        <v>1500</v>
+        <v>13000</v>
       </c>
       <c r="AV4">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="AW4">
         <v>5</v>
@@ -1430,40 +1430,40 @@
         <v>5</v>
       </c>
       <c r="AZ4">
-        <v>0.0641025641025641</v>
+        <v>0.1</v>
       </c>
       <c r="BA4">
         <v>1</v>
       </c>
       <c r="BC4">
-        <v>0.9358974358974359</v>
+        <v>0.9</v>
       </c>
       <c r="BD4">
-        <v>1600</v>
+        <v>13200</v>
       </c>
       <c r="BE4">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="BF4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BI4">
-        <v>0.05714285714285714</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="BJ4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="BL4">
-        <v>0.9428571428571428</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="BM4">
-        <v>1500</v>
+        <v>18600</v>
       </c>
       <c r="BN4">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="BO4">
         <v>5</v>
@@ -1472,19 +1472,19 @@
         <v>5</v>
       </c>
       <c r="BR4">
-        <v>0.06172839506172839</v>
+        <v>0.09433962264150944</v>
       </c>
       <c r="BS4">
         <v>1</v>
       </c>
       <c r="BU4">
-        <v>0.9382716049382716</v>
+        <v>0.9056603773584906</v>
       </c>
       <c r="BV4">
-        <v>1500</v>
+        <v>20600</v>
       </c>
       <c r="BW4">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="BX4">
         <v>5</v>
@@ -1493,19 +1493,19 @@
         <v>5</v>
       </c>
       <c r="CA4">
-        <v>0.05952380952380952</v>
+        <v>0.09259259259259259</v>
       </c>
       <c r="CB4">
         <v>1</v>
       </c>
       <c r="CD4">
-        <v>0.9404761904761905</v>
+        <v>0.9074074074074074</v>
       </c>
       <c r="CE4">
-        <v>2800</v>
+        <v>15200</v>
       </c>
       <c r="CF4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="CG4">
         <v>5</v>
@@ -1514,46 +1514,46 @@
         <v>5</v>
       </c>
       <c r="CJ4">
-        <v>0.1</v>
+        <v>0.09803921568627451</v>
       </c>
       <c r="CK4">
         <v>1</v>
       </c>
       <c r="CM4">
-        <v>0.9</v>
+        <v>0.9019607843137255</v>
       </c>
       <c r="CN4">
-        <v>1930</v>
+        <v>15750</v>
       </c>
       <c r="CO4">
-        <v>73.5</v>
+        <v>53.9</v>
       </c>
       <c r="CP4">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CQ4">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CR4" t="str">
         <v/>
       </c>
       <c r="CS4">
-        <v>0.06924729263724617</v>
+        <v>0.09312290473959106</v>
       </c>
       <c r="CT4">
-        <v>0.9800000000000001</v>
+        <v>1</v>
       </c>
       <c r="CU4" t="str">
         <v/>
       </c>
       <c r="CV4">
-        <v>0.9307527073627538</v>
+        <v>0.906877095260409</v>
       </c>
       <c r="CW4">
-        <v>1400</v>
+        <v>7600</v>
       </c>
       <c r="CX4">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="CY4">
         <v>5</v>
@@ -1579,262 +1579,262 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>79100</v>
+        <v>19200</v>
       </c>
       <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="K5">
+        <v>14300</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="Q5">
+        <v>0.8</v>
+      </c>
+      <c r="S5">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="T5">
+        <v>16900</v>
+      </c>
+      <c r="U5">
+        <v>11</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="Y5">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>0.5454545454545454</v>
+      </c>
+      <c r="AC5">
+        <v>18600</v>
+      </c>
+      <c r="AD5">
+        <v>16</v>
+      </c>
+      <c r="AE5">
+        <v>5</v>
+      </c>
+      <c r="AF5">
+        <v>5</v>
+      </c>
+      <c r="AH5">
+        <v>0.3125</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>0.6875</v>
+      </c>
+      <c r="AL5">
+        <v>16400</v>
+      </c>
+      <c r="AM5">
+        <v>15</v>
+      </c>
+      <c r="AN5">
+        <v>4</v>
+      </c>
+      <c r="AO5">
+        <v>4</v>
+      </c>
+      <c r="AQ5">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="AR5">
+        <v>0.8</v>
+      </c>
+      <c r="AT5">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="AU5">
+        <v>16100</v>
+      </c>
+      <c r="AV5">
+        <v>13</v>
+      </c>
+      <c r="AW5">
+        <v>5</v>
+      </c>
+      <c r="AX5">
+        <v>5</v>
+      </c>
+      <c r="AZ5">
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="BA5">
+        <v>1</v>
+      </c>
+      <c r="BC5">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="BD5">
+        <v>22000</v>
+      </c>
+      <c r="BE5">
+        <v>14</v>
+      </c>
+      <c r="BF5">
+        <v>4</v>
+      </c>
+      <c r="BG5">
+        <v>4</v>
+      </c>
+      <c r="BI5">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="BJ5">
+        <v>0.8</v>
+      </c>
+      <c r="BL5">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="BM5">
+        <v>14300</v>
+      </c>
+      <c r="BN5">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0.1</v>
-      </c>
-      <c r="H5">
-        <v>0.2</v>
-      </c>
-      <c r="J5">
-        <v>0.9</v>
-      </c>
-      <c r="K5">
-        <v>106600</v>
-      </c>
-      <c r="L5">
-        <v>9</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>13000</v>
-      </c>
-      <c r="U5">
-        <v>29</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>0.034482758620689655</v>
-      </c>
-      <c r="Z5">
-        <v>0.2</v>
-      </c>
-      <c r="AB5">
-        <v>0.9655172413793104</v>
-      </c>
-      <c r="AC5">
-        <v>14200</v>
-      </c>
-      <c r="AD5">
-        <v>32</v>
-      </c>
-      <c r="AE5">
-        <v>2</v>
-      </c>
-      <c r="AF5">
-        <v>2</v>
-      </c>
-      <c r="AH5">
-        <v>0.0625</v>
-      </c>
-      <c r="AI5">
-        <v>0.4</v>
-      </c>
-      <c r="AK5">
-        <v>0.9375</v>
-      </c>
-      <c r="AL5">
-        <v>17800</v>
-      </c>
-      <c r="AM5">
-        <v>18</v>
-      </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
-      <c r="AQ5">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="AR5">
-        <v>0.2</v>
-      </c>
-      <c r="AT5">
-        <v>0.9444444444444444</v>
-      </c>
-      <c r="AU5">
-        <v>29800</v>
-      </c>
-      <c r="AV5">
+      <c r="BO5">
+        <v>5</v>
+      </c>
+      <c r="BP5">
+        <v>5</v>
+      </c>
+      <c r="BR5">
+        <v>0.5</v>
+      </c>
+      <c r="BS5">
+        <v>1</v>
+      </c>
+      <c r="BU5">
+        <v>0.5</v>
+      </c>
+      <c r="BV5">
+        <v>12900</v>
+      </c>
+      <c r="BW5">
         <v>10</v>
       </c>
-      <c r="AW5">
-        <v>0</v>
-      </c>
-      <c r="AX5">
-        <v>0</v>
-      </c>
-      <c r="AZ5">
-        <v>0</v>
-      </c>
-      <c r="BA5">
-        <v>0</v>
-      </c>
-      <c r="BC5">
-        <v>1</v>
-      </c>
-      <c r="BD5">
-        <v>19200</v>
-      </c>
-      <c r="BE5">
-        <v>27</v>
-      </c>
-      <c r="BF5">
-        <v>0</v>
-      </c>
-      <c r="BG5">
-        <v>0</v>
-      </c>
-      <c r="BI5">
-        <v>0</v>
-      </c>
-      <c r="BJ5">
-        <v>0</v>
-      </c>
-      <c r="BL5">
-        <v>1</v>
-      </c>
-      <c r="BM5">
-        <v>27800</v>
-      </c>
-      <c r="BN5">
-        <v>22</v>
-      </c>
-      <c r="BO5">
-        <v>1</v>
-      </c>
-      <c r="BP5">
-        <v>1</v>
-      </c>
-      <c r="BR5">
-        <v>0.045454545454545456</v>
-      </c>
-      <c r="BS5">
-        <v>0.2</v>
-      </c>
-      <c r="BU5">
-        <v>0.9545454545454546</v>
-      </c>
-      <c r="BV5">
-        <v>13800</v>
-      </c>
-      <c r="BW5">
-        <v>22</v>
-      </c>
       <c r="BX5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BY5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="CA5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="CB5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="CE5">
-        <v>17200</v>
+        <v>14100</v>
       </c>
       <c r="CF5">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="CG5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CH5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CJ5">
-        <v>0.03225806451612903</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="CK5">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="CM5">
-        <v>0.967741935483871</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="CN5">
-        <v>33850</v>
+        <v>16480</v>
       </c>
       <c r="CO5">
-        <v>21</v>
+        <v>12.4</v>
       </c>
       <c r="CP5">
-        <v>0.7</v>
+        <v>4.7</v>
       </c>
       <c r="CQ5">
-        <v>0.7</v>
+        <v>4.7</v>
       </c>
       <c r="CR5" t="str">
         <v/>
       </c>
       <c r="CS5">
-        <v>0.03302509241469197</v>
+        <v>0.39500735375735374</v>
       </c>
       <c r="CT5">
-        <v>0.13999999999999999</v>
+        <v>0.9399999999999998</v>
       </c>
       <c r="CU5" t="str">
         <v/>
       </c>
       <c r="CV5">
-        <v>0.966974907585308</v>
+        <v>0.6049926462426463</v>
       </c>
       <c r="CW5">
-        <v>13000</v>
+        <v>12900</v>
       </c>
       <c r="CX5">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="CY5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="CZ5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="DB5">
-        <v>0.1</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="DC5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="DE5">
-        <v>0.9</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="DF5">
         <v>100</v>
@@ -1845,10 +1845,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1400</v>
+        <v>34100</v>
       </c>
       <c r="C6">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1857,19 +1857,19 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>0.058823529411764705</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0.9411764705882353</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="K6">
-        <v>1500</v>
+        <v>9800</v>
       </c>
       <c r="L6">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="M6">
         <v>5</v>
@@ -1878,19 +1878,19 @@
         <v>5</v>
       </c>
       <c r="P6">
-        <v>0.06097560975609756</v>
+        <v>0.07936507936507936</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="S6">
-        <v>0.9390243902439024</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="T6">
-        <v>1400</v>
+        <v>8400</v>
       </c>
       <c r="U6">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="V6">
         <v>5</v>
@@ -1899,19 +1899,19 @@
         <v>5</v>
       </c>
       <c r="Y6">
-        <v>0.06097560975609756</v>
+        <v>0.08928571428571429</v>
       </c>
       <c r="Z6">
         <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.9390243902439024</v>
+        <v>0.9107142857142857</v>
       </c>
       <c r="AC6">
-        <v>1400</v>
+        <v>6100</v>
       </c>
       <c r="AD6">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="AE6">
         <v>5</v>
@@ -1920,19 +1920,19 @@
         <v>5</v>
       </c>
       <c r="AH6">
-        <v>0.06097560975609756</v>
+        <v>0.078125</v>
       </c>
       <c r="AI6">
         <v>1</v>
       </c>
       <c r="AK6">
-        <v>0.9390243902439024</v>
+        <v>0.921875</v>
       </c>
       <c r="AL6">
-        <v>1500</v>
+        <v>12900</v>
       </c>
       <c r="AM6">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="AN6">
         <v>5</v>
@@ -1941,19 +1941,19 @@
         <v>5</v>
       </c>
       <c r="AQ6">
-        <v>0.060240963855421686</v>
+        <v>0.08771929824561403</v>
       </c>
       <c r="AR6">
         <v>1</v>
       </c>
       <c r="AT6">
-        <v>0.9397590361445783</v>
+        <v>0.9122807017543859</v>
       </c>
       <c r="AU6">
-        <v>1500</v>
+        <v>12900</v>
       </c>
       <c r="AV6">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="AW6">
         <v>5</v>
@@ -1962,40 +1962,40 @@
         <v>5</v>
       </c>
       <c r="AZ6">
-        <v>0.06097560975609756</v>
+        <v>0.08620689655172414</v>
       </c>
       <c r="BA6">
         <v>1</v>
       </c>
       <c r="BC6">
-        <v>0.9390243902439024</v>
+        <v>0.9137931034482759</v>
       </c>
       <c r="BD6">
-        <v>3300</v>
+        <v>16000</v>
       </c>
       <c r="BE6">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="BF6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BG6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BI6">
-        <v>0.047619047619047616</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="BJ6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="BL6">
-        <v>0.9523809523809523</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="BM6">
-        <v>1400</v>
+        <v>18300</v>
       </c>
       <c r="BN6">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="BO6">
         <v>5</v>
@@ -2004,19 +2004,19 @@
         <v>5</v>
       </c>
       <c r="BR6">
-        <v>0.06172839506172839</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="BS6">
         <v>1</v>
       </c>
       <c r="BU6">
-        <v>0.9382716049382716</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="BV6">
-        <v>1400</v>
+        <v>9500</v>
       </c>
       <c r="BW6">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="BX6">
         <v>5</v>
@@ -2025,19 +2025,19 @@
         <v>5</v>
       </c>
       <c r="CA6">
-        <v>0.05952380952380952</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="CB6">
         <v>1</v>
       </c>
       <c r="CD6">
-        <v>0.9404761904761905</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="CE6">
-        <v>4100</v>
+        <v>10900</v>
       </c>
       <c r="CF6">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="CG6">
         <v>5</v>
@@ -2046,46 +2046,46 @@
         <v>5</v>
       </c>
       <c r="CJ6">
-        <v>0.06097560975609756</v>
+        <v>0.078125</v>
       </c>
       <c r="CK6">
         <v>1</v>
       </c>
       <c r="CM6">
-        <v>0.9390243902439024</v>
+        <v>0.921875</v>
       </c>
       <c r="CN6">
-        <v>1890</v>
+        <v>13890</v>
       </c>
       <c r="CO6">
-        <v>82.7</v>
+        <v>59.6</v>
       </c>
       <c r="CP6">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CQ6">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="CR6" t="str">
         <v/>
       </c>
       <c r="CS6">
-        <v>0.059281379425225975</v>
+        <v>0.08411485087357538</v>
       </c>
       <c r="CT6">
-        <v>0.9800000000000001</v>
+        <v>1</v>
       </c>
       <c r="CU6" t="str">
         <v/>
       </c>
       <c r="CV6">
-        <v>0.940718620574774</v>
+        <v>0.9158851491264246</v>
       </c>
       <c r="CW6">
-        <v>1400</v>
+        <v>6100</v>
       </c>
       <c r="CX6">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="CY6">
         <v>5</v>
@@ -2094,13 +2094,13 @@
         <v>5</v>
       </c>
       <c r="DB6">
-        <v>0.06172839506172839</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="DC6">
         <v>1</v>
       </c>
       <c r="DE6">
-        <v>0.9382716049382716</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="DF6">
         <v>100</v>

</xml_diff>